<commit_message>
Refined compute_bio_avgcon, add demflag in fix death
Former-commit-id: a9b0d81ed92680d4548ea6f9d4b431e84cb445b1
Former-commit-id: 1dd046362a7c3ef7d39a8ff55485cbb699559cfc [formerly a07890bd643f9e4d1b25114b9e34f6213b161b09] [formerly 2721d7f3049d71f2082376457e693540cd193173 [formerly d1a3324c307665dc49625344b897e393cbe92a32]] [formerly 204ff123b3fa8f8dd7a82fa9ae3da722a09f7603 [formerly e2e593f4cb1fcbbde7ff80f307d3d4ab70b5f4c6] [formerly b0f01376e9a02f72d744b3d689695ad745b71629 [formerly b7438df9be044ef3c5ff3e8f21aadbd7609bc249]]]
Former-commit-id: ccc8358b7c1b2415961a11d4e8840975b92b83e0 [formerly 6ebcb836c17657693e49507d018800050b382b5b] [formerly 84f4ff3e149a66d75cd229f8a213c3a9344c9b0c [formerly 82f46b96543e476a438aae4337bb9d2a8d34ed61]]
Former-commit-id: 4042aa62ff8f72f9b344e76b5b9a700b2846479a [formerly 1af71249447c3b956996b3de1b229488f5a5fc50]
Former-commit-id: 814cedad5babe199a46711b1dc2db3f247a00aef
</commit_message>
<xml_diff>
--- a/code/examples/nitrify/tcase1-rbulk/AOBNOB-run1.xlsx
+++ b/code/examples/nitrify/tcase1-rbulk/AOBNOB-run1.xlsx
@@ -5,29 +5,64 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Downloads\NUFeb2Lit\Test Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Downloads\Code versions\IbM- JAN2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Reactions" sheetId="18" r:id="rId1"/>
     <sheet name="SpecParam" sheetId="13" r:id="rId2"/>
     <sheet name="ReactionMatrix" sheetId="21" r:id="rId3"/>
-    <sheet name="States" sheetId="22" r:id="rId4"/>
-    <sheet name="ThermoParam" sheetId="24" r:id="rId5"/>
-    <sheet name="Bacteria" sheetId="25" r:id="rId6"/>
-    <sheet name="Parameters" sheetId="26" r:id="rId7"/>
-    <sheet name="Discretization" sheetId="27" r:id="rId8"/>
-    <sheet name="Diffusion" sheetId="28" r:id="rId9"/>
+    <sheet name="Influent" sheetId="29" r:id="rId4"/>
+    <sheet name="States" sheetId="22" r:id="rId5"/>
+    <sheet name="ThermoParam" sheetId="24" r:id="rId6"/>
+    <sheet name="Bacteria" sheetId="25" r:id="rId7"/>
+    <sheet name="Parameters" sheetId="26" r:id="rId8"/>
+    <sheet name="Discretization" sheetId="27" r:id="rId9"/>
+    <sheet name="Diffusion" sheetId="28" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>R.Gonzalez-Cabaleiro</author>
+  </authors>
+  <commentList>
+    <comment ref="D4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>R.Gonzalez-Cabaleiro:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Si es dirichlet == states</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="141">
   <si>
     <t>P</t>
   </si>
@@ -707,7 +742,10 @@
     <t>DECAY</t>
   </si>
   <si>
-    <t>Na</t>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Tol</t>
   </si>
 </sst>
 </file>
@@ -724,7 +762,7 @@
     <numFmt numFmtId="170" formatCode="0.0"/>
     <numFmt numFmtId="171" formatCode="0.0000E+00"/>
   </numFmts>
-  <fonts count="39" x14ac:knownFonts="1">
+  <fonts count="41" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -973,6 +1011,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -1591,7 +1642,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="262">
+  <cellXfs count="265">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1"/>
@@ -2230,6 +2281,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2782,30 +2842,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:40" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="S2" s="248" t="s">
+      <c r="S2" s="251" t="s">
         <v>22</v>
       </c>
-      <c r="T2" s="248"/>
-      <c r="U2" s="248"/>
-      <c r="V2" s="248"/>
-      <c r="W2" s="248" t="s">
+      <c r="T2" s="251"/>
+      <c r="U2" s="251"/>
+      <c r="V2" s="251"/>
+      <c r="W2" s="251" t="s">
         <v>23</v>
       </c>
-      <c r="X2" s="248"/>
-      <c r="Y2" s="248"/>
-      <c r="Z2" s="248"/>
-      <c r="AA2" s="248" t="s">
+      <c r="X2" s="251"/>
+      <c r="Y2" s="251"/>
+      <c r="Z2" s="251"/>
+      <c r="AA2" s="251" t="s">
         <v>74</v>
       </c>
-      <c r="AB2" s="248"/>
-      <c r="AC2" s="248"/>
-      <c r="AD2" s="248"/>
-      <c r="AE2" s="248" t="s">
+      <c r="AB2" s="251"/>
+      <c r="AC2" s="251"/>
+      <c r="AD2" s="251"/>
+      <c r="AE2" s="251" t="s">
         <v>76</v>
       </c>
-      <c r="AF2" s="248"/>
-      <c r="AG2" s="248"/>
-      <c r="AH2" s="248"/>
+      <c r="AF2" s="251"/>
+      <c r="AG2" s="251"/>
+      <c r="AH2" s="251"/>
       <c r="AK2" s="3" t="s">
         <v>24</v>
       </c>
@@ -4165,10 +4225,10 @@
         <f>1/F16</f>
         <v>3.4893748785390075E-2</v>
       </c>
-      <c r="J16" s="249" t="s">
+      <c r="J16" s="252" t="s">
         <v>56</v>
       </c>
-      <c r="K16" s="252" t="s">
+      <c r="K16" s="255" t="s">
         <v>57</v>
       </c>
       <c r="R16" s="47" t="s">
@@ -4268,8 +4328,8 @@
         <f t="shared" ref="G17:G18" si="11">1/F17</f>
         <v>2.1521507799447302E-2</v>
       </c>
-      <c r="J17" s="250"/>
-      <c r="K17" s="253"/>
+      <c r="J17" s="253"/>
+      <c r="K17" s="256"/>
       <c r="R17" s="50" t="s">
         <v>59</v>
       </c>
@@ -4367,8 +4427,8 @@
         <f t="shared" si="11"/>
         <v>5.6574173051404053E-2</v>
       </c>
-      <c r="J18" s="250"/>
-      <c r="K18" s="253"/>
+      <c r="J18" s="253"/>
+      <c r="K18" s="256"/>
       <c r="R18" s="50" t="s">
         <v>60</v>
       </c>
@@ -4449,8 +4509,8 @@
       <c r="E19" s="31"/>
       <c r="F19" s="40"/>
       <c r="G19" s="63"/>
-      <c r="J19" s="250"/>
-      <c r="K19" s="253"/>
+      <c r="J19" s="253"/>
+      <c r="K19" s="256"/>
       <c r="R19" s="50" t="s">
         <v>61</v>
       </c>
@@ -4531,8 +4591,8 @@
       <c r="E20" s="31"/>
       <c r="F20" s="31"/>
       <c r="G20" s="65"/>
-      <c r="J20" s="250"/>
-      <c r="K20" s="253"/>
+      <c r="J20" s="253"/>
+      <c r="K20" s="256"/>
       <c r="R20" s="50" t="s">
         <v>62</v>
       </c>
@@ -4613,8 +4673,8 @@
       <c r="E21" s="31"/>
       <c r="F21" s="31"/>
       <c r="G21" s="65"/>
-      <c r="J21" s="250"/>
-      <c r="K21" s="253"/>
+      <c r="J21" s="253"/>
+      <c r="K21" s="256"/>
       <c r="R21" s="50" t="s">
         <v>63</v>
       </c>
@@ -4695,8 +4755,8 @@
       <c r="E22" s="31"/>
       <c r="F22" s="31"/>
       <c r="G22" s="65"/>
-      <c r="J22" s="250"/>
-      <c r="K22" s="253"/>
+      <c r="J22" s="253"/>
+      <c r="K22" s="256"/>
       <c r="R22" s="52" t="s">
         <v>38</v>
       </c>
@@ -4777,8 +4837,8 @@
       <c r="E23" s="31"/>
       <c r="F23" s="31"/>
       <c r="G23" s="65"/>
-      <c r="J23" s="250"/>
-      <c r="K23" s="253"/>
+      <c r="J23" s="253"/>
+      <c r="K23" s="256"/>
       <c r="V23" s="55" t="s">
         <v>64</v>
       </c>
@@ -4799,8 +4859,8 @@
       <c r="E24" s="31"/>
       <c r="F24" s="31"/>
       <c r="G24" s="65"/>
-      <c r="J24" s="250"/>
-      <c r="K24" s="253"/>
+      <c r="J24" s="253"/>
+      <c r="K24" s="256"/>
     </row>
     <row r="25" spans="2:36" ht="18" x14ac:dyDescent="0.25">
       <c r="B25" s="64"/>
@@ -4809,14 +4869,14 @@
       <c r="E25" s="31"/>
       <c r="F25" s="31"/>
       <c r="G25" s="65"/>
-      <c r="J25" s="250"/>
-      <c r="K25" s="253"/>
-      <c r="N25" s="255" t="s">
+      <c r="J25" s="253"/>
+      <c r="K25" s="256"/>
+      <c r="N25" s="258" t="s">
         <v>65</v>
       </c>
-      <c r="O25" s="256"/>
-      <c r="P25" s="256"/>
-      <c r="Q25" s="257"/>
+      <c r="O25" s="259"/>
+      <c r="P25" s="259"/>
+      <c r="Q25" s="260"/>
       <c r="R25" s="56" t="s">
         <v>66</v>
       </c>
@@ -4892,14 +4952,14 @@
       <c r="E26" s="31"/>
       <c r="F26" s="31"/>
       <c r="G26" s="65"/>
-      <c r="J26" s="250"/>
-      <c r="K26" s="253"/>
-      <c r="N26" s="255" t="s">
+      <c r="J26" s="253"/>
+      <c r="K26" s="256"/>
+      <c r="N26" s="258" t="s">
         <v>67</v>
       </c>
-      <c r="O26" s="256"/>
-      <c r="P26" s="256"/>
-      <c r="Q26" s="257"/>
+      <c r="O26" s="259"/>
+      <c r="P26" s="259"/>
+      <c r="Q26" s="260"/>
       <c r="R26" s="59" t="s">
         <v>68</v>
       </c>
@@ -4975,8 +5035,8 @@
       <c r="E27" s="31"/>
       <c r="F27" s="31"/>
       <c r="G27" s="65"/>
-      <c r="J27" s="250"/>
-      <c r="K27" s="253"/>
+      <c r="J27" s="253"/>
+      <c r="K27" s="256"/>
       <c r="O27" s="33"/>
       <c r="P27" s="33"/>
       <c r="Q27" s="33"/>
@@ -4988,8 +5048,8 @@
       <c r="E28" s="31"/>
       <c r="F28" s="31"/>
       <c r="G28" s="65"/>
-      <c r="J28" s="250"/>
-      <c r="K28" s="253"/>
+      <c r="J28" s="253"/>
+      <c r="K28" s="256"/>
     </row>
     <row r="29" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B29" s="62"/>
@@ -4998,8 +5058,8 @@
       <c r="E29" s="62"/>
       <c r="F29" s="62"/>
       <c r="G29" s="63"/>
-      <c r="J29" s="250"/>
-      <c r="K29" s="253"/>
+      <c r="J29" s="253"/>
+      <c r="K29" s="256"/>
     </row>
     <row r="30" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B30" s="62"/>
@@ -5008,8 +5068,8 @@
       <c r="E30" s="62"/>
       <c r="F30" s="62"/>
       <c r="G30" s="63"/>
-      <c r="J30" s="250"/>
-      <c r="K30" s="253"/>
+      <c r="J30" s="253"/>
+      <c r="K30" s="256"/>
     </row>
     <row r="31" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B31" s="62"/>
@@ -5018,8 +5078,8 @@
       <c r="E31" s="62"/>
       <c r="F31" s="62"/>
       <c r="G31" s="63"/>
-      <c r="J31" s="250"/>
-      <c r="K31" s="253"/>
+      <c r="J31" s="253"/>
+      <c r="K31" s="256"/>
     </row>
     <row r="32" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="62"/>
@@ -5028,8 +5088,8 @@
       <c r="E32" s="62"/>
       <c r="F32" s="62"/>
       <c r="G32" s="63"/>
-      <c r="J32" s="251"/>
-      <c r="K32" s="254"/>
+      <c r="J32" s="254"/>
+      <c r="K32" s="257"/>
     </row>
     <row r="33" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B33" s="62"/>
@@ -5223,6 +5283,113 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="68"/>
+    <col min="2" max="2" width="12" style="68" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="68"/>
+    <col min="5" max="5" width="12.42578125" style="68" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="68"/>
+    <col min="7" max="7" width="11.42578125" style="68" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="68"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="213" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="214">
+        <f>1.957*10^(-9)*3600</f>
+        <v>7.0452000000000007E-6</v>
+      </c>
+      <c r="C1" s="215" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="164" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="109">
+        <f>1.912*10^(-9)*3600</f>
+        <v>6.8832000000000004E-6</v>
+      </c>
+      <c r="C2" s="216" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="164" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="109">
+        <f>1.902*10^(-9)*3600</f>
+        <v>6.8471999999999994E-6</v>
+      </c>
+      <c r="C3" s="216" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="164" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="217">
+        <f>2.1*10^(-9)*3600</f>
+        <v>7.5600000000000005E-6</v>
+      </c>
+      <c r="C4" s="216" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="164" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="217">
+        <f>1.185*10^(-9)*3600</f>
+        <v>4.2660000000000003E-6</v>
+      </c>
+      <c r="C5" s="216" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="159" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="218">
+        <v>0</v>
+      </c>
+      <c r="C6" s="219" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="184" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" s="220">
+        <v>0</v>
+      </c>
+      <c r="C7" s="221" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L24"/>
@@ -5442,13 +5609,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5467,22 +5634,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B1" s="258" t="s">
+      <c r="B1" s="261" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="259"/>
-      <c r="D1" s="260"/>
-      <c r="E1" s="258" t="s">
+      <c r="C1" s="262"/>
+      <c r="D1" s="263"/>
+      <c r="E1" s="261" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="259"/>
-      <c r="G1" s="260"/>
-      <c r="H1" s="261"/>
-      <c r="I1" s="261"/>
-      <c r="J1" s="261"/>
-      <c r="K1" s="261"/>
-      <c r="L1" s="261"/>
-      <c r="M1" s="261"/>
+      <c r="F1" s="262"/>
+      <c r="G1" s="263"/>
+      <c r="H1" s="264"/>
+      <c r="I1" s="264"/>
+      <c r="J1" s="264"/>
+      <c r="K1" s="264"/>
+      <c r="L1" s="264"/>
+      <c r="M1" s="264"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B2" s="69" t="s">
@@ -5687,9 +5854,10 @@
     </row>
     <row r="8" spans="1:13" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="77" t="s">
-        <v>139</v>
+        <v>7</v>
       </c>
       <c r="B8" s="78">
+        <f>Reactions!S10</f>
         <v>0</v>
       </c>
       <c r="C8" s="79">
@@ -5699,9 +5867,11 @@
         <v>0</v>
       </c>
       <c r="E8" s="78">
+        <f>Reactions!W10</f>
         <v>0</v>
       </c>
       <c r="F8" s="79">
+        <f>Reactions!Z10</f>
         <v>0</v>
       </c>
       <c r="G8" s="80">
@@ -5716,10 +5886,10 @@
     </row>
     <row r="9" spans="1:13" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="77" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B9" s="78">
-        <f>Reactions!S10</f>
+        <f>Reactions!S11</f>
         <v>0</v>
       </c>
       <c r="C9" s="79">
@@ -5729,11 +5899,11 @@
         <v>0</v>
       </c>
       <c r="E9" s="78">
-        <f>Reactions!W10</f>
+        <f>Reactions!W11</f>
         <v>0</v>
       </c>
       <c r="F9" s="79">
-        <f>Reactions!Z10</f>
+        <f>Reactions!Z11</f>
         <v>0</v>
       </c>
       <c r="G9" s="80">
@@ -5747,28 +5917,25 @@
       <c r="M9" s="76"/>
     </row>
     <row r="10" spans="1:13" s="81" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="77" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="78">
-        <f>Reactions!S11</f>
-        <v>0</v>
-      </c>
-      <c r="C10" s="79">
-        <v>0</v>
-      </c>
-      <c r="D10" s="80">
-        <v>0</v>
-      </c>
-      <c r="E10" s="78">
-        <f>Reactions!W11</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="79">
-        <f>Reactions!Z11</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="80">
+      <c r="A10" s="82" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="83">
+        <v>0</v>
+      </c>
+      <c r="C10" s="84">
+        <v>0</v>
+      </c>
+      <c r="D10" s="85">
+        <v>0</v>
+      </c>
+      <c r="E10" s="83">
+        <v>0</v>
+      </c>
+      <c r="F10" s="84">
+        <v>0</v>
+      </c>
+      <c r="G10" s="85">
         <v>0</v>
       </c>
       <c r="H10" s="76"/>
@@ -5778,27 +5945,33 @@
       <c r="L10" s="76"/>
       <c r="M10" s="76"/>
     </row>
-    <row r="11" spans="1:13" s="81" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="82" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="83">
-        <v>0</v>
-      </c>
-      <c r="C11" s="84">
-        <v>0</v>
-      </c>
-      <c r="D11" s="85">
-        <v>0</v>
-      </c>
-      <c r="E11" s="83">
-        <v>0</v>
-      </c>
-      <c r="F11" s="84">
-        <v>0</v>
-      </c>
-      <c r="G11" s="85">
-        <v>0</v>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="77" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="86">
+        <f>Reactions!S12</f>
+        <v>1</v>
+      </c>
+      <c r="C11" s="79">
+        <f>Reactions!V12</f>
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="D11" s="87">
+        <f>Reactions!AI12</f>
+        <v>-2.5</v>
+      </c>
+      <c r="E11" s="74">
+        <f>Reactions!W12</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="236">
+        <f>Reactions!Z12</f>
+        <v>0.19999999999999973</v>
+      </c>
+      <c r="G11" s="237">
+        <f>Reactions!AI12</f>
+        <v>-2.5</v>
       </c>
       <c r="H11" s="76"/>
       <c r="I11" s="76"/>
@@ -5808,32 +5981,32 @@
       <c r="M11" s="76"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="77" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="86">
-        <f>Reactions!S12</f>
+      <c r="A12" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="88">
+        <f>Reactions!S13</f>
         <v>1</v>
       </c>
-      <c r="C12" s="79">
-        <f>Reactions!V12</f>
-        <v>1.0999999999999999</v>
-      </c>
-      <c r="D12" s="87">
-        <f>Reactions!AI12</f>
-        <v>-2.5</v>
-      </c>
-      <c r="E12" s="74">
-        <f>Reactions!W12</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="236">
-        <f>Reactions!Z12</f>
-        <v>0.19999999999999973</v>
-      </c>
-      <c r="G12" s="237">
-        <f>Reactions!AI12</f>
-        <v>-2.5</v>
+      <c r="C12" s="84">
+        <f>Reactions!V13</f>
+        <v>-1</v>
+      </c>
+      <c r="D12" s="89">
+        <f>Reactions!AI13</f>
+        <v>1</v>
+      </c>
+      <c r="E12" s="83">
+        <f>Reactions!W13</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="84">
+        <f>Reactions!Z13</f>
+        <v>-1</v>
+      </c>
+      <c r="G12" s="89">
+        <f>Reactions!AI13</f>
+        <v>1</v>
       </c>
       <c r="H12" s="76"/>
       <c r="I12" s="76"/>
@@ -5843,63 +6016,59 @@
       <c r="M12" s="76"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="88">
-        <f>Reactions!S13</f>
+      <c r="A13" s="73" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="86">
+        <v>0</v>
+      </c>
+      <c r="C13" s="90">
         <v>1</v>
       </c>
-      <c r="C13" s="84">
-        <f>Reactions!V13</f>
+      <c r="D13" s="87">
+        <f t="shared" ref="D13:D14" si="0">-C13</f>
         <v>-1</v>
       </c>
-      <c r="D13" s="89">
-        <f>Reactions!AI13</f>
+      <c r="E13" s="86">
+        <v>0</v>
+      </c>
+      <c r="F13" s="90">
+        <v>0</v>
+      </c>
+      <c r="G13" s="87">
+        <f t="shared" ref="G13:G14" si="1">-F13</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="91"/>
+      <c r="I13" s="91"/>
+      <c r="J13" s="91"/>
+      <c r="K13" s="91"/>
+      <c r="L13" s="91"/>
+      <c r="M13" s="91"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="82" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="88">
+        <v>0</v>
+      </c>
+      <c r="C14" s="92">
+        <v>0</v>
+      </c>
+      <c r="D14" s="89">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="88">
+        <v>0</v>
+      </c>
+      <c r="F14" s="92">
         <v>1</v>
       </c>
-      <c r="E13" s="83">
-        <f>Reactions!W13</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="84">
-        <f>Reactions!Z13</f>
+      <c r="G14" s="89">
+        <f t="shared" si="1"/>
         <v>-1</v>
-      </c>
-      <c r="G13" s="89">
-        <f>Reactions!AI13</f>
-        <v>1</v>
-      </c>
-      <c r="H13" s="76"/>
-      <c r="I13" s="76"/>
-      <c r="J13" s="76"/>
-      <c r="K13" s="76"/>
-      <c r="L13" s="76"/>
-      <c r="M13" s="76"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="73" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="86">
-        <v>0</v>
-      </c>
-      <c r="C14" s="90">
-        <v>1</v>
-      </c>
-      <c r="D14" s="87">
-        <f t="shared" ref="D14:D15" si="0">-C14</f>
-        <v>-1</v>
-      </c>
-      <c r="E14" s="86">
-        <v>0</v>
-      </c>
-      <c r="F14" s="90">
-        <v>0</v>
-      </c>
-      <c r="G14" s="87">
-        <f t="shared" ref="G14:G15" si="1">-F14</f>
-        <v>0</v>
       </c>
       <c r="H14" s="91"/>
       <c r="I14" s="91"/>
@@ -5908,39 +6077,8 @@
       <c r="L14" s="91"/>
       <c r="M14" s="91"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="82" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="88">
-        <v>0</v>
-      </c>
-      <c r="C15" s="92">
-        <v>0</v>
-      </c>
-      <c r="D15" s="89">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="88">
-        <v>0</v>
-      </c>
-      <c r="F15" s="92">
-        <v>1</v>
-      </c>
-      <c r="G15" s="89">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-      <c r="H15" s="91"/>
-      <c r="I15" s="91"/>
-      <c r="J15" s="91"/>
-      <c r="K15" s="91"/>
-      <c r="L15" s="91"/>
-      <c r="M15" s="91"/>
-    </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I21" s="93"/>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I20" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5949,27 +6087,27 @@
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B14:D14 G4:G8 H3:M14 B3:C13 D4:D13 E3:F13">
+  <conditionalFormatting sqref="B13:D13 G4:G7 H3:M13 B3:C12 D4:D12 E3:F12">
     <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:D15">
+  <conditionalFormatting sqref="B14:D14">
     <cfRule type="cellIs" dxfId="14" priority="20" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14:F14">
+  <conditionalFormatting sqref="E13:F13">
     <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15:F15">
+  <conditionalFormatting sqref="E14:F14">
     <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H15:J15">
+  <conditionalFormatting sqref="H14:J14">
     <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -5979,17 +6117,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K15:M15">
+  <conditionalFormatting sqref="K14:M14">
     <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G9:G14">
+  <conditionalFormatting sqref="G8:G13">
     <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G15">
+  <conditionalFormatting sqref="G14">
     <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -6005,11 +6143,99 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="108" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="117">
+        <f>30/(17*1000)</f>
+        <v>1.7647058823529412E-3</v>
+      </c>
+      <c r="C1" s="248" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="122" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="112" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="109">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="C2" s="249" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="250" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="112" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="109">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="C3" s="249" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="250" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="112" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="109">
+        <f>5/(32*1000)</f>
+        <v>1.5625E-4</v>
+      </c>
+      <c r="C4" s="249" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="250" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="112" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="109">
+        <v>1E-3</v>
+      </c>
+      <c r="C5" s="249" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="250" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6027,8 +6253,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="109">
-        <f>Parameters!B1</f>
-        <v>2.941176470588235E-4</v>
+        <v>1.75E-3</v>
       </c>
       <c r="C1" s="110" t="s">
         <v>85</v>
@@ -6042,8 +6267,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="109">
-        <f>0.006</f>
-        <v>6.0000000000000001E-3</v>
+        <v>9.9999999999999995E-21</v>
       </c>
       <c r="C2" s="113" t="s">
         <v>85</v>
@@ -6072,8 +6296,8 @@
         <v>12</v>
       </c>
       <c r="B4" s="109">
-        <f>9/32/1000</f>
-        <v>2.8124999999999998E-4</v>
+        <f>5/32/1000</f>
+        <v>1.5625E-4</v>
       </c>
       <c r="C4" s="113" t="s">
         <v>85</v>
@@ -6103,7 +6327,7 @@
       </c>
       <c r="B6" s="117">
         <f>B4/(1.34*10^(-3))</f>
-        <v>0.20988805970149252</v>
+        <v>0.1166044776119403</v>
       </c>
       <c r="C6" s="110" t="s">
         <v>87</v>
@@ -6133,7 +6357,7 @@
       </c>
       <c r="B8" s="116">
         <f>1-SUM(B6:B7)</f>
-        <v>0.78949429323968401</v>
+        <v>0.88277787532923613</v>
       </c>
       <c r="C8" s="119" t="s">
         <v>87</v>
@@ -6183,7 +6407,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
@@ -6879,7 +7103,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
@@ -7023,7 +7247,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
@@ -7170,12 +7394,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7324,6 +7548,17 @@
         <v>114</v>
       </c>
     </row>
+    <row r="13" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="211" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" s="246">
+        <v>1</v>
+      </c>
+      <c r="C13" s="247" t="s">
+        <v>101</v>
+      </c>
+    </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="212"/>
       <c r="E16" s="126"/>
@@ -7334,113 +7569,6 @@
     </row>
     <row r="28" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E28" s="115"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="68"/>
-    <col min="2" max="2" width="12" style="68" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="68"/>
-    <col min="5" max="5" width="12.42578125" style="68" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="68"/>
-    <col min="7" max="7" width="11.42578125" style="68" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="68"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="213" t="s">
-        <v>129</v>
-      </c>
-      <c r="B1" s="214">
-        <f>1.957*10^(-9)*3600</f>
-        <v>7.0452000000000007E-6</v>
-      </c>
-      <c r="C1" s="215" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="164" t="s">
-        <v>131</v>
-      </c>
-      <c r="B2" s="109">
-        <f>1.912*10^(-9)*3600</f>
-        <v>6.8832000000000004E-6</v>
-      </c>
-      <c r="C2" s="216" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="164" t="s">
-        <v>132</v>
-      </c>
-      <c r="B3" s="109">
-        <f>1.902*10^(-9)*3600</f>
-        <v>6.8471999999999994E-6</v>
-      </c>
-      <c r="C3" s="216" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="164" t="s">
-        <v>133</v>
-      </c>
-      <c r="B4" s="217">
-        <f>2.1*10^(-9)*3600</f>
-        <v>7.5600000000000005E-6</v>
-      </c>
-      <c r="C4" s="216" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="164" t="s">
-        <v>134</v>
-      </c>
-      <c r="B5" s="217">
-        <f>1.185*10^(-9)*3600</f>
-        <v>4.2660000000000003E-6</v>
-      </c>
-      <c r="C5" s="216" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="159" t="s">
-        <v>135</v>
-      </c>
-      <c r="B6" s="218">
-        <v>0</v>
-      </c>
-      <c r="C6" s="219" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="184" t="s">
-        <v>137</v>
-      </c>
-      <c r="B7" s="220">
-        <v>0</v>
-      </c>
-      <c r="C7" s="221" t="s">
-        <v>136</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>